<commit_message>
review down ch 4
</commit_message>
<xml_diff>
--- a/indicators/NO_GJEN_002/metadata.xlsx
+++ b/indicators/NO_GJEN_002/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\41001581_egenutvikling_anders_kolstad\github\ecRxiv_encroachment_reviewALK\indicators\NO_GJEN_002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D22C0E9-285F-4A6A-A1AC-D1520B1DC123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A348CAC-9BB2-47A6-A8EF-74B91B5C8304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="2670" windowWidth="21600" windowHeight="12615" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
+    <workbookView xWindow="16800" yWindow="2670" windowWidth="21600" windowHeight="12615" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -570,13 +570,13 @@
     <t>NO_GJEN_002</t>
   </si>
   <si>
-    <t>Gray, A.</t>
-  </si>
-  <si>
     <t>First draft. NO_GJEN_002 is also related to and a continuation of NO_GJEN_001 which is based LiDAR</t>
   </si>
   <si>
     <t>https://github.com/NINAnor/ecRxiv/tree/indicators/NO_GJEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gray, A., Mienna, I. M., Venter, Z., </t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1206,7 @@
         <v>159</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1216,7 +1216,7 @@
         <v>174</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1226,7 +1226,7 @@
         <v>173</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>

</xml_diff>